<commit_message>
Add geochemical soil survey NL
</commit_message>
<xml_diff>
--- a/output/reprojected_polder_data.xlsx
+++ b/output/reprojected_polder_data.xlsx
@@ -1045,334 +1045,334 @@
     <t>wpxtra 1m B T</t>
   </si>
   <si>
-    <t>POINT (650786.2464680928 6885812.586896558)</t>
-  </si>
-  <si>
-    <t>POINT (651894.4825726995 6887235.298555037)</t>
-  </si>
-  <si>
-    <t>POINT (631822.1417841916 6878055.230200602)</t>
-  </si>
-  <si>
-    <t>POINT (631657.7821120179 6878055.884592394)</t>
-  </si>
-  <si>
-    <t>POINT (632503.7056526174 6888007.48048795)</t>
-  </si>
-  <si>
-    <t>POINT (632487.2493623364 6888007.547576849)</t>
-  </si>
-  <si>
-    <t>POINT (631717.705383289 6887750.637739368)</t>
-  </si>
-  <si>
-    <t>POINT (631716.0598059476 6887750.6442887895)</t>
-  </si>
-  <si>
-    <t>POINT (660779.3183178427 6885591.580651903)</t>
-  </si>
-  <si>
-    <t>POINT (658899.1081426805 6885623.729513086)</t>
-  </si>
-  <si>
-    <t>POINT (662850.7493539307 6885819.082394737)</t>
-  </si>
-  <si>
-    <t>POINT (662867.2006905742 6885818.953272207)</t>
-  </si>
-  <si>
-    <t>POINT (648739.3188747525 6901165.176710194)</t>
-  </si>
-  <si>
-    <t>POINT (648739.3088234458 6901163.528410285)</t>
-  </si>
-  <si>
-    <t>POINT (651628.9345387137 6884589.821193228)</t>
-  </si>
-  <si>
-    <t>POINT (651790.1350825747 6884588.779312476)</t>
-  </si>
-  <si>
-    <t>POINT (654088.4709180001 6894617.452217638)</t>
-  </si>
-  <si>
-    <t>POINT (654088.4820535277 6894619.099167924)</t>
-  </si>
-  <si>
-    <t>POINT (630903.5278156842 6896765.268726382)</t>
-  </si>
-  <si>
-    <t>POINT (631262.4678542548 6895454.253963909)</t>
-  </si>
-  <si>
-    <t>POINT (627322.1392433867 6882912.21817465)</t>
-  </si>
-  <si>
-    <t>POINT (627125.3170264955 6882585.620353284)</t>
-  </si>
-  <si>
-    <t>POINT (639798.0298312898 6902698.3963617105)</t>
-  </si>
-  <si>
-    <t>POINT (639814.5161055208 6902698.314131074)</t>
-  </si>
-  <si>
-    <t>POINT (623622.7808753886 6844055.484563485)</t>
-  </si>
-  <si>
-    <t>POINT (622533.6980640789 6845548.17729116)</t>
-  </si>
-  <si>
-    <t>POINT (639557.0575374895 6871422.563169483)</t>
-  </si>
-  <si>
-    <t>POINT (639422.5239744168 6871449.504573588)</t>
-  </si>
-  <si>
-    <t>POINT (629858.6037864573 6847117.042654197)</t>
-  </si>
-  <si>
-    <t>POINT (629887.9156513029 6847074.3626168175)</t>
-  </si>
-  <si>
-    <t>POINT (624811.4590703091 6843145.187948278)</t>
-  </si>
-  <si>
-    <t>POINT (624813.0955672998 6843145.182847288)</t>
-  </si>
-  <si>
-    <t>POINT (619027.4140972253 6843571.916948595)</t>
-  </si>
-  <si>
-    <t>POINT (618998.8226262622 6841884.830314618)</t>
-  </si>
-  <si>
-    <t>POINT (627750.3559306372 6848706.467726416)</t>
-  </si>
-  <si>
-    <t>POINT (627738.921064858 6848714.695758773)</t>
-  </si>
-  <si>
-    <t>POINT (637329.1604652201 6855415.689658398)</t>
-  </si>
-  <si>
-    <t>POINT (637329.16812207 6855417.328635846)</t>
-  </si>
-  <si>
-    <t>POINT (624443.40485739 6858660.661509362)</t>
-  </si>
-  <si>
-    <t>POINT (626182.8894762024 6858599.379804738)</t>
-  </si>
-  <si>
-    <t>POINT (632015.1153749432 6859817.7604676485)</t>
-  </si>
-  <si>
-    <t>POINT (631838.0280555513 6859823.388878135)</t>
-  </si>
-  <si>
-    <t>POINT (612149.8555157806 6850606.275022324)</t>
-  </si>
-  <si>
-    <t>POINT (612149.8301782944 6850589.894837412)</t>
-  </si>
-  <si>
-    <t>POINT (615154.3498754905 6847379.718630455)</t>
-  </si>
-  <si>
-    <t>POINT (615046.5429271793 6847515.827626682)</t>
-  </si>
-  <si>
-    <t>POINT (608660.4861916584 6853207.604057717)</t>
-  </si>
-  <si>
-    <t>POINT (608660.467937963 6853191.218572761)</t>
-  </si>
-  <si>
-    <t>POINT (607868.7118403557 6852859.443142777)</t>
-  </si>
-  <si>
-    <t>POINT (607867.0733607284 6852859.444806904)</t>
-  </si>
-  <si>
-    <t>POINT (638862.7106414264 6858670.674769487)</t>
-  </si>
-  <si>
-    <t>POINT (638700.3865048984 6858671.462454493)</t>
-  </si>
-  <si>
-    <t>POINT (632198.5002912073 6842693.297169053)</t>
-  </si>
-  <si>
-    <t>POINT (632196.8638929026 6842693.303768688)</t>
-  </si>
-  <si>
-    <t>POINT (564591.5888895027 6918490.371498683)</t>
-  </si>
-  <si>
-    <t>POINT (562939.7315095988 6918479.688106614)</t>
-  </si>
-  <si>
-    <t>POINT (564184.7322829454 6917104.407710172)</t>
-  </si>
-  <si>
-    <t>POINT (564052.1513856278 6917206.222421963)</t>
-  </si>
-  <si>
-    <t>POINT (568027.1141880923 6908955.677622048)</t>
-  </si>
-  <si>
-    <t>POINT (568027.0492469635 6908972.1768434495)</t>
-  </si>
-  <si>
-    <t>POINT (558215.3713765166 6921344.754190781)</t>
-  </si>
-  <si>
-    <t>POINT (558215.3799004626 6921343.101738252)</t>
-  </si>
-  <si>
-    <t>POINT (561800.3181996377 6915940.778253664)</t>
-  </si>
-  <si>
-    <t>POINT (561801.0962074423 6915775.645242449)</t>
-  </si>
-  <si>
-    <t>POINT (550894.2548993153 6907012.374623039)</t>
-  </si>
-  <si>
-    <t>POINT (552541.6501455882 6906537.24272937)</t>
-  </si>
-  <si>
-    <t>POINT (563630.5226015913 6908103.991852495)</t>
-  </si>
-  <si>
-    <t>POINT (563526.0252824926 6908228.9065566)</t>
-  </si>
-  <si>
-    <t>POINT (561658.5046929332 6916595.734906507)</t>
-  </si>
-  <si>
-    <t>POINT (561656.923506299 6916580.863777193)</t>
-  </si>
-  <si>
-    <t>POINT (565987.1137058334 6925667.158879593)</t>
-  </si>
-  <si>
-    <t>POINT (565988.7670570472 6925667.165810666)</t>
-  </si>
-  <si>
-    <t>POINT (567783.7039193974 6917913.961476444)</t>
-  </si>
-  <si>
-    <t>POINT (566171.4029992243 6917555.5803947)</t>
-  </si>
-  <si>
-    <t>POINT (565019.5471161997 6922295.814725481)</t>
-  </si>
-  <si>
-    <t>POINT (565016.1919129657 6922307.3690778185)</t>
-  </si>
-  <si>
-    <t>POINT (557976.9263298567 6907750.013986221)</t>
-  </si>
-  <si>
-    <t>POINT (557976.9177756517 6907751.663647342)</t>
-  </si>
-  <si>
-    <t>POINT (608327.9250805442 6839529.476515237)</t>
-  </si>
-  <si>
-    <t>POINT (607092.4760638818 6840831.251975645)</t>
-  </si>
-  <si>
-    <t>POINT (601854.9059225518 6826422.300072547)</t>
-  </si>
-  <si>
-    <t>POINT (601309.7514469102 6827943.004055552)</t>
-  </si>
-  <si>
-    <t>POINT (594010.0746288248 6825476.71179399)</t>
-  </si>
-  <si>
-    <t>POINT (594510.3798322884 6827041.543079308)</t>
-  </si>
-  <si>
-    <t>POINT (594030.0324088925 6824959.10479718)</t>
-  </si>
-  <si>
-    <t>POINT (595534.1803312879 6824337.937417271)</t>
-  </si>
-  <si>
-    <t>POINT (596825.2168961616 6820930.149456345)</t>
-  </si>
-  <si>
-    <t>POINT (596986.7843912605 6820933.469063375)</t>
-  </si>
-  <si>
-    <t>POINT (599588.2241068962 6819135.647732114)</t>
-  </si>
-  <si>
-    <t>POINT (599770.9693192092 6819243.336959521)</t>
-  </si>
-  <si>
-    <t>POINT (607978.5984596167 6835469.238615422)</t>
-  </si>
-  <si>
-    <t>POINT (608074.9141276991 6835328.5344192125)</t>
-  </si>
-  <si>
-    <t>POINT (603116.5195819533 6839929.2472601915)</t>
-  </si>
-  <si>
-    <t>POINT (603208.0673500998 6839791.79712062)</t>
-  </si>
-  <si>
-    <t>POINT (604793.7235195715 6832903.7871513795)</t>
-  </si>
-  <si>
-    <t>POINT (604805.1717946685 6832915.220908703)</t>
-  </si>
-  <si>
-    <t>POINT (609936.203946678 6830774.4094128795)</t>
-  </si>
-  <si>
-    <t>POINT (609952.5439167006 6830774.388624065)</t>
-  </si>
-  <si>
-    <t>POINT (586532.1132754266 6825961.14678148)</t>
-  </si>
-  <si>
-    <t>POINT (586532.1398948386 6825944.81658633)</t>
-  </si>
-  <si>
-    <t>POINT (598055.834047391 6836712.729917548)</t>
-  </si>
-  <si>
-    <t>POINT (598055.8307490128 6836729.081956357)</t>
-  </si>
-  <si>
-    <t>POINT (596726.3337596373 6836933.107475961)</t>
-  </si>
-  <si>
-    <t>POINT (596727.969006476 6836933.108075241)</t>
-  </si>
-  <si>
-    <t>POINT (605535.8116705157 6826227.763510216)</t>
-  </si>
-  <si>
-    <t>POINT (605535.8104855964 6826226.130432984)</t>
-  </si>
-  <si>
-    <t>POINT (600115.7141596015 6827879.453226768)</t>
-  </si>
-  <si>
-    <t>POINT (600114.0807472114 6827879.453314338)</t>
-  </si>
-  <si>
-    <t>POINT (593021.3229984895 6828461.497419653)</t>
-  </si>
-  <si>
-    <t>POINT (593022.9565280195 6828461.498768406)</t>
+    <t>POINT (5.846112318970617 52.65701914821788)</t>
+  </si>
+  <si>
+    <t>POINT (5.8560677732824304 52.66479009862622)</t>
+  </si>
+  <si>
+    <t>POINT (5.675754868098707 52.61462349689506)</t>
+  </si>
+  <si>
+    <t>POINT (5.674278400042641 52.61462707503078)</t>
+  </si>
+  <si>
+    <t>POINT (5.681877460499812 52.669007228992086)</t>
+  </si>
+  <si>
+    <t>POINT (5.681729631129018 52.66900759536806)</t>
+  </si>
+  <si>
+    <t>POINT (5.674816699947214 52.667604574699354)</t>
+  </si>
+  <si>
+    <t>POINT (5.674801917474444 52.667604610467244)</t>
+  </si>
+  <si>
+    <t>POINT (5.9358816107499655 52.65581187208736)</t>
+  </si>
+  <si>
+    <t>POINT (5.918991395372913 52.65598749161802)</t>
+  </si>
+  <si>
+    <t>POINT (5.95448959234714 52.65705463023741)</t>
+  </si>
+  <si>
+    <t>POINT (5.954637377218651 52.6570539248987)</t>
+  </si>
+  <si>
+    <t>POINT (5.827724455544781 52.74080273858885)</t>
+  </si>
+  <si>
+    <t>POINT (5.827724365252357 52.7407937520058)</t>
+  </si>
+  <si>
+    <t>POINT (5.8536823147064565 52.650339207109866)</t>
+  </si>
+  <si>
+    <t>POINT (5.855130403830043 52.65033351490178)</t>
+  </si>
+  <si>
+    <t>POINT (5.8757767059200665 52.70508964820048)</t>
+  </si>
+  <si>
+    <t>POINT (5.875776805952213 52.7050986348158)</t>
+  </si>
+  <si>
+    <t>POINT (5.667502818417548 52.71680766935835)</t>
+  </si>
+  <si>
+    <t>POINT (5.670727231644851 52.70965543315031)</t>
+  </si>
+  <si>
+    <t>POINT (5.635330657488889 52.64117283118716)</t>
+  </si>
+  <si>
+    <t>POINT (5.6335625734320125 52.63938808530209)</t>
+  </si>
+  <si>
+    <t>POINT (5.747403489470051 52.74916109401226)</t>
+  </si>
+  <si>
+    <t>POINT (5.747551588191251 52.74916064577468)</t>
+  </si>
+  <si>
+    <t>POINT (5.602098755854809 52.428320073511365)</t>
+  </si>
+  <si>
+    <t>POINT (5.592315358504094 52.43651603250899)</t>
+  </si>
+  <si>
+    <t>POINT (5.745238798524349 52.57834177200539)</t>
+  </si>
+  <si>
+    <t>POINT (5.744030262964997 52.57848920677466)</t>
+  </si>
+  <si>
+    <t>POINT (5.658116106155565 52.445128583203314)</t>
+  </si>
+  <si>
+    <t>POINT (5.658379419117534 52.44489430633676)</t>
+  </si>
+  <si>
+    <t>POINT (5.612776833758774 52.4233211370272)</t>
+  </si>
+  <si>
+    <t>POINT (5.6127915346613655 52.42332110901328)</t>
+  </si>
+  <si>
+    <t>POINT (5.560817873725216 52.42566461024887)</t>
+  </si>
+  <si>
+    <t>POINT (5.5605610321715995 52.41639888357573)</t>
+  </si>
+  <si>
+    <t>POINT (5.639177393439611 52.453852274568106)</t>
+  </si>
+  <si>
+    <t>POINT (5.6390746722925975 52.45389743028845)</t>
+  </si>
+  <si>
+    <t>POINT (5.7252252586097025 52.49065726287612)</t>
+  </si>
+  <si>
+    <t>POINT (5.725225327392356 52.49066625008681)</t>
+  </si>
+  <si>
+    <t>POINT (5.609470546510277 52.50844720874757)</t>
+  </si>
+  <si>
+    <t>POINT (5.625096602705977 52.50811131038396)</t>
+  </si>
+  <si>
+    <t>POINT (5.677488379358743 52.51478903579811)</t>
+  </si>
+  <si>
+    <t>POINT (5.6758975769024085 52.51481988173804)</t>
+  </si>
+  <si>
+    <t>POINT (5.499035713813825 52.4642772463945)</t>
+  </si>
+  <si>
+    <t>POINT (5.499035486203314 52.464187372634534)</t>
+  </si>
+  <si>
+    <t>POINT (5.526025545857608 52.44657042186665)</t>
+  </si>
+  <si>
+    <t>POINT (5.525057099563585 52.447317510792494)</t>
+  </si>
+  <si>
+    <t>POINT (5.467690175855856 52.47854771373215)</t>
+  </si>
+  <si>
+    <t>POINT (5.467690011880121 52.478457840184284)</t>
+  </si>
+  <si>
+    <t>POINT (5.460577545842366 52.47663802921268)</t>
+  </si>
+  <si>
+    <t>POINT (5.460562827129448 52.47663803834072)</t>
+  </si>
+  <si>
+    <t>POINT (5.739001374232205 52.5085020933609)</t>
+  </si>
+  <si>
+    <t>POINT (5.73754319170396 52.508506410811684)</t>
+  </si>
+  <si>
+    <t>POINT (5.6791357540903125 52.42083934604499)</t>
+  </si>
+  <si>
+    <t>POINT (5.6791210540742325 52.42083938229131)</t>
+  </si>
+  <si>
+    <t>POINT (5.0718125358476565 52.835157406714806)</t>
+  </si>
+  <si>
+    <t>POINT (5.056973648532123 52.835099287289246)</t>
+  </si>
+  <si>
+    <t>POINT (5.068157680766503 52.82761688114269)</t>
+  </si>
+  <si>
+    <t>POINT (5.0669666863020755 52.82817086277342)</t>
+  </si>
+  <si>
+    <t>POINT (5.10267438469468 52.78325599507085)</t>
+  </si>
+  <si>
+    <t>POINT (5.102673801318594 52.78334586116521)</t>
+  </si>
+  <si>
+    <t>POINT (5.014533999379798 52.850682922506486)</t>
+  </si>
+  <si>
+    <t>POINT (5.0145340759517065 52.85067393612504)</t>
+  </si>
+  <si>
+    <t>POINT (5.046738124619451 52.82128498012977)</t>
+  </si>
+  <si>
+    <t>POINT (5.046745113582472 52.8203863321109)</t>
+  </si>
+  <si>
+    <t>POINT (4.948767291096905 52.772670127312324)</t>
+  </si>
+  <si>
+    <t>POINT (4.963566094384033 52.770081519999074)</t>
+  </si>
+  <si>
+    <t>POINT (5.063179130492828 52.77861687599245)</t>
+  </si>
+  <si>
+    <t>POINT (5.06224041510387 52.77929731553227)</t>
+  </si>
+  <si>
+    <t>POINT (5.045464192213778 52.82484904720382)</t>
+  </si>
+  <si>
+    <t>POINT (5.045449988172574 52.824768126478084)</t>
+  </si>
+  <si>
+    <t>POINT (5.084348748566437 52.87418266324956)</t>
+  </si>
+  <si>
+    <t>POINT (5.084363600873091 52.874182700921665)</t>
+  </si>
+  <si>
+    <t>POINT (5.100487793047877 52.832021528907575)</t>
+  </si>
+  <si>
+    <t>POINT (5.086004247455962 52.83007169224504)</t>
+  </si>
+  <si>
+    <t>POINT (5.075656950007723 52.85585467786636)</t>
+  </si>
+  <si>
+    <t>POINT (5.075626809704259 52.85591750526866)</t>
+  </si>
+  <si>
+    <t>POINT (5.012392011081426 52.77668861789061)</t>
+  </si>
+  <si>
+    <t>POINT (5.0123919342376935 52.77669760444939)</t>
+  </si>
+  <si>
+    <t>POINT (5.46470272856568 52.403459662410285)</t>
+  </si>
+  <si>
+    <t>POINT (5.4536045012214975 52.410611484467815)</t>
+  </si>
+  <si>
+    <t>POINT (5.406554608125449 52.33138521651187)</t>
+  </si>
+  <si>
+    <t>POINT (5.401657402148699 52.33975340617269)</t>
+  </si>
+  <si>
+    <t>POINT (5.336083289600509 52.326180993749134)</t>
+  </si>
+  <si>
+    <t>POINT (5.340577607710467 52.334793003337516)</t>
+  </si>
+  <si>
+    <t>POINT (5.336262573389228 52.32333198578596)</t>
+  </si>
+  <si>
+    <t>POINT (5.349774564071872 52.319912718248375)</t>
+  </si>
+  <si>
+    <t>POINT (5.361372142857704 52.301149540964694)</t>
+  </si>
+  <si>
+    <t>POINT (5.362823528360347 52.30116782250991)</t>
+  </si>
+  <si>
+    <t>POINT (5.386192658933058 52.291265855867444)</t>
+  </si>
+  <si>
+    <t>POINT (5.387834287106262 52.2918590448272)</t>
+  </si>
+  <si>
+    <t>POINT (5.4615646741383905 52.38114564204505)</t>
+  </si>
+  <si>
+    <t>POINT (5.462429892505776 52.38037216480185)</t>
+  </si>
+  <si>
+    <t>POINT (5.417887876454393 52.405656086229605)</t>
+  </si>
+  <si>
+    <t>POINT (5.418710264047924 52.40490091890363)</t>
+  </si>
+  <si>
+    <t>POINT (5.432954455771871 52.367040736821025)</t>
+  </si>
+  <si>
+    <t>POINT (5.433057297376837 52.36710360989914)</t>
+  </si>
+  <si>
+    <t>POINT (5.479150143431424 52.35532993541956)</t>
+  </si>
+  <si>
+    <t>POINT (5.479296927879559 52.355329821073425)</t>
+  </si>
+  <si>
+    <t>POINT (5.268907619822382 52.32884724959388)</t>
+  </si>
+  <si>
+    <t>POINT (5.268907858948628 52.328757373335584)</t>
+  </si>
+  <si>
+    <t>POINT (5.372426964816193 52.38798075401587)</t>
+  </si>
+  <si>
+    <t>POINT (5.3724269351863585 52.388070629358296)</t>
+  </si>
+  <si>
+    <t>POINT (5.360483860528889 52.389191994761966)</t>
+  </si>
+  <si>
+    <t>POINT (5.360498550201175 52.38919199805569)</t>
+  </si>
+  <si>
+    <t>POINT (5.439620747053444 52.33031459826143)</t>
+  </si>
+  <si>
+    <t>POINT (5.4396207364091325 52.33030561062583)</t>
+  </si>
+  <si>
+    <t>POINT (5.390931182698719 52.33940372803456)</t>
+  </si>
+  <si>
+    <t>POINT (5.3909165095055664 52.33940372851641)</t>
+  </si>
+  <si>
+    <t>POINT (5.327201182583226 52.342606228068114)</t>
+  </si>
+  <si>
+    <t>POINT (5.327215856828666 52.3426062354889)</t>
   </si>
 </sst>
 </file>
@@ -1797,10 +1797,10 @@
         <v>343</v>
       </c>
       <c r="J2">
-        <v>650786.2464680928</v>
+        <v>5.846112318970617</v>
       </c>
       <c r="K2">
-        <v>6885812.586896558</v>
+        <v>52.65701914821788</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1832,10 +1832,10 @@
         <v>343</v>
       </c>
       <c r="J3">
-        <v>650786.2464680928</v>
+        <v>5.846112318970617</v>
       </c>
       <c r="K3">
-        <v>6885812.586896558</v>
+        <v>52.65701914821788</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1867,10 +1867,10 @@
         <v>343</v>
       </c>
       <c r="J4">
-        <v>650786.2464680928</v>
+        <v>5.846112318970617</v>
       </c>
       <c r="K4">
-        <v>6885812.586896558</v>
+        <v>52.65701914821788</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1902,10 +1902,10 @@
         <v>344</v>
       </c>
       <c r="J5">
-        <v>651894.4825726995</v>
+        <v>5.85606777328243</v>
       </c>
       <c r="K5">
-        <v>6887235.298555037</v>
+        <v>52.66479009862622</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1937,10 +1937,10 @@
         <v>344</v>
       </c>
       <c r="J6">
-        <v>651894.4825726995</v>
+        <v>5.85606777328243</v>
       </c>
       <c r="K6">
-        <v>6887235.298555037</v>
+        <v>52.66479009862622</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1972,10 +1972,10 @@
         <v>345</v>
       </c>
       <c r="J7">
-        <v>631822.1417841916</v>
+        <v>5.675754868098707</v>
       </c>
       <c r="K7">
-        <v>6878055.230200602</v>
+        <v>52.61462349689506</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -2007,10 +2007,10 @@
         <v>345</v>
       </c>
       <c r="J8">
-        <v>631822.1417841916</v>
+        <v>5.675754868098707</v>
       </c>
       <c r="K8">
-        <v>6878055.230200602</v>
+        <v>52.61462349689506</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -2042,10 +2042,10 @@
         <v>346</v>
       </c>
       <c r="J9">
-        <v>631657.7821120179</v>
+        <v>5.674278400042641</v>
       </c>
       <c r="K9">
-        <v>6878055.884592394</v>
+        <v>52.61462707503078</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -2077,10 +2077,10 @@
         <v>346</v>
       </c>
       <c r="J10">
-        <v>631657.7821120179</v>
+        <v>5.674278400042641</v>
       </c>
       <c r="K10">
-        <v>6878055.884592394</v>
+        <v>52.61462707503078</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2112,10 +2112,10 @@
         <v>346</v>
       </c>
       <c r="J11">
-        <v>631657.7821120179</v>
+        <v>5.674278400042641</v>
       </c>
       <c r="K11">
-        <v>6878055.884592394</v>
+        <v>52.61462707503078</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2147,10 +2147,10 @@
         <v>347</v>
       </c>
       <c r="J12">
-        <v>632503.7056526174</v>
+        <v>5.681877460499812</v>
       </c>
       <c r="K12">
-        <v>6888007.48048795</v>
+        <v>52.66900722899209</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -2182,10 +2182,10 @@
         <v>347</v>
       </c>
       <c r="J13">
-        <v>632503.7056526174</v>
+        <v>5.681877460499812</v>
       </c>
       <c r="K13">
-        <v>6888007.48048795</v>
+        <v>52.66900722899209</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2217,10 +2217,10 @@
         <v>347</v>
       </c>
       <c r="J14">
-        <v>632503.7056526174</v>
+        <v>5.681877460499812</v>
       </c>
       <c r="K14">
-        <v>6888007.48048795</v>
+        <v>52.66900722899209</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -2252,10 +2252,10 @@
         <v>348</v>
       </c>
       <c r="J15">
-        <v>632487.2493623364</v>
+        <v>5.681729631129018</v>
       </c>
       <c r="K15">
-        <v>6888007.547576849</v>
+        <v>52.66900759536806</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2287,10 +2287,10 @@
         <v>348</v>
       </c>
       <c r="J16">
-        <v>632487.2493623364</v>
+        <v>5.681729631129018</v>
       </c>
       <c r="K16">
-        <v>6888007.547576849</v>
+        <v>52.66900759536806</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -2322,10 +2322,10 @@
         <v>349</v>
       </c>
       <c r="J17">
-        <v>631717.705383289</v>
+        <v>5.674816699947214</v>
       </c>
       <c r="K17">
-        <v>6887750.637739368</v>
+        <v>52.66760457469935</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -2357,10 +2357,10 @@
         <v>349</v>
       </c>
       <c r="J18">
-        <v>631717.705383289</v>
+        <v>5.674816699947214</v>
       </c>
       <c r="K18">
-        <v>6887750.637739368</v>
+        <v>52.66760457469935</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -2392,10 +2392,10 @@
         <v>350</v>
       </c>
       <c r="J19">
-        <v>631716.0598059476</v>
+        <v>5.674801917474444</v>
       </c>
       <c r="K19">
-        <v>6887750.644288789</v>
+        <v>52.66760461046724</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -2427,10 +2427,10 @@
         <v>350</v>
       </c>
       <c r="J20">
-        <v>631716.0598059476</v>
+        <v>5.674801917474444</v>
       </c>
       <c r="K20">
-        <v>6887750.644288789</v>
+        <v>52.66760461046724</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -2462,10 +2462,10 @@
         <v>351</v>
       </c>
       <c r="J21">
-        <v>660779.3183178427</v>
+        <v>5.935881610749965</v>
       </c>
       <c r="K21">
-        <v>6885591.580651903</v>
+        <v>52.65581187208736</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -2497,10 +2497,10 @@
         <v>351</v>
       </c>
       <c r="J22">
-        <v>660779.3183178427</v>
+        <v>5.935881610749965</v>
       </c>
       <c r="K22">
-        <v>6885591.580651903</v>
+        <v>52.65581187208736</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -2532,10 +2532,10 @@
         <v>352</v>
       </c>
       <c r="J23">
-        <v>658899.1081426805</v>
+        <v>5.918991395372913</v>
       </c>
       <c r="K23">
-        <v>6885623.729513086</v>
+        <v>52.65598749161802</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -2567,10 +2567,10 @@
         <v>352</v>
       </c>
       <c r="J24">
-        <v>658899.1081426805</v>
+        <v>5.918991395372913</v>
       </c>
       <c r="K24">
-        <v>6885623.729513086</v>
+        <v>52.65598749161802</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -2602,10 +2602,10 @@
         <v>353</v>
       </c>
       <c r="J25">
-        <v>662850.7493539307</v>
+        <v>5.95448959234714</v>
       </c>
       <c r="K25">
-        <v>6885819.082394737</v>
+        <v>52.65705463023741</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -2637,10 +2637,10 @@
         <v>353</v>
       </c>
       <c r="J26">
-        <v>662850.7493539307</v>
+        <v>5.95448959234714</v>
       </c>
       <c r="K26">
-        <v>6885819.082394737</v>
+        <v>52.65705463023741</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -2672,10 +2672,10 @@
         <v>354</v>
       </c>
       <c r="J27">
-        <v>662867.2006905742</v>
+        <v>5.954637377218651</v>
       </c>
       <c r="K27">
-        <v>6885818.953272207</v>
+        <v>52.6570539248987</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -2707,10 +2707,10 @@
         <v>354</v>
       </c>
       <c r="J28">
-        <v>662867.2006905742</v>
+        <v>5.954637377218651</v>
       </c>
       <c r="K28">
-        <v>6885818.953272207</v>
+        <v>52.6570539248987</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -2742,10 +2742,10 @@
         <v>355</v>
       </c>
       <c r="J29">
-        <v>648739.3188747525</v>
+        <v>5.827724455544781</v>
       </c>
       <c r="K29">
-        <v>6901165.176710194</v>
+        <v>52.74080273858885</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -2777,10 +2777,10 @@
         <v>355</v>
       </c>
       <c r="J30">
-        <v>648739.3188747525</v>
+        <v>5.827724455544781</v>
       </c>
       <c r="K30">
-        <v>6901165.176710194</v>
+        <v>52.74080273858885</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -2812,10 +2812,10 @@
         <v>355</v>
       </c>
       <c r="J31">
-        <v>648739.3188747525</v>
+        <v>5.827724455544781</v>
       </c>
       <c r="K31">
-        <v>6901165.176710194</v>
+        <v>52.74080273858885</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -2847,10 +2847,10 @@
         <v>356</v>
       </c>
       <c r="J32">
-        <v>648739.3088234458</v>
+        <v>5.827724365252357</v>
       </c>
       <c r="K32">
-        <v>6901163.528410285</v>
+        <v>52.7407937520058</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -2882,10 +2882,10 @@
         <v>356</v>
       </c>
       <c r="J33">
-        <v>648739.3088234458</v>
+        <v>5.827724365252357</v>
       </c>
       <c r="K33">
-        <v>6901163.528410285</v>
+        <v>52.7407937520058</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -2917,10 +2917,10 @@
         <v>357</v>
       </c>
       <c r="J34">
-        <v>651628.9345387137</v>
+        <v>5.853682314706457</v>
       </c>
       <c r="K34">
-        <v>6884589.821193228</v>
+        <v>52.65033920710987</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -2952,10 +2952,10 @@
         <v>357</v>
       </c>
       <c r="J35">
-        <v>651628.9345387137</v>
+        <v>5.853682314706457</v>
       </c>
       <c r="K35">
-        <v>6884589.821193228</v>
+        <v>52.65033920710987</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -2987,10 +2987,10 @@
         <v>358</v>
       </c>
       <c r="J36">
-        <v>651790.1350825747</v>
+        <v>5.855130403830043</v>
       </c>
       <c r="K36">
-        <v>6884588.779312476</v>
+        <v>52.65033351490178</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -3022,10 +3022,10 @@
         <v>358</v>
       </c>
       <c r="J37">
-        <v>651790.1350825747</v>
+        <v>5.855130403830043</v>
       </c>
       <c r="K37">
-        <v>6884588.779312476</v>
+        <v>52.65033351490178</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -3057,10 +3057,10 @@
         <v>358</v>
       </c>
       <c r="J38">
-        <v>651790.1350825747</v>
+        <v>5.855130403830043</v>
       </c>
       <c r="K38">
-        <v>6884588.779312476</v>
+        <v>52.65033351490178</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -3092,10 +3092,10 @@
         <v>358</v>
       </c>
       <c r="J39">
-        <v>651790.1350825747</v>
+        <v>5.855130403830043</v>
       </c>
       <c r="K39">
-        <v>6884588.779312476</v>
+        <v>52.65033351490178</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -3127,10 +3127,10 @@
         <v>359</v>
       </c>
       <c r="J40">
-        <v>654088.4709180001</v>
+        <v>5.875776705920067</v>
       </c>
       <c r="K40">
-        <v>6894617.452217638</v>
+        <v>52.70508964820048</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -3162,10 +3162,10 @@
         <v>359</v>
       </c>
       <c r="J41">
-        <v>654088.4709180001</v>
+        <v>5.875776705920067</v>
       </c>
       <c r="K41">
-        <v>6894617.452217638</v>
+        <v>52.70508964820048</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -3197,10 +3197,10 @@
         <v>360</v>
       </c>
       <c r="J42">
-        <v>654088.4820535277</v>
+        <v>5.875776805952213</v>
       </c>
       <c r="K42">
-        <v>6894619.099167924</v>
+        <v>52.7050986348158</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -3232,10 +3232,10 @@
         <v>360</v>
       </c>
       <c r="J43">
-        <v>654088.4820535277</v>
+        <v>5.875776805952213</v>
       </c>
       <c r="K43">
-        <v>6894619.099167924</v>
+        <v>52.7050986348158</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -3267,10 +3267,10 @@
         <v>360</v>
       </c>
       <c r="J44">
-        <v>654088.4820535277</v>
+        <v>5.875776805952213</v>
       </c>
       <c r="K44">
-        <v>6894619.099167924</v>
+        <v>52.7050986348158</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -3302,10 +3302,10 @@
         <v>361</v>
       </c>
       <c r="J45">
-        <v>630903.5278156842</v>
+        <v>5.667502818417548</v>
       </c>
       <c r="K45">
-        <v>6896765.268726382</v>
+        <v>52.71680766935835</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -3337,10 +3337,10 @@
         <v>361</v>
       </c>
       <c r="J46">
-        <v>630903.5278156842</v>
+        <v>5.667502818417548</v>
       </c>
       <c r="K46">
-        <v>6896765.268726382</v>
+        <v>52.71680766935835</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -3372,10 +3372,10 @@
         <v>362</v>
       </c>
       <c r="J47">
-        <v>631262.4678542548</v>
+        <v>5.670727231644851</v>
       </c>
       <c r="K47">
-        <v>6895454.253963909</v>
+        <v>52.70965543315031</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -3407,10 +3407,10 @@
         <v>362</v>
       </c>
       <c r="J48">
-        <v>631262.4678542548</v>
+        <v>5.670727231644851</v>
       </c>
       <c r="K48">
-        <v>6895454.253963909</v>
+        <v>52.70965543315031</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -3442,10 +3442,10 @@
         <v>363</v>
       </c>
       <c r="J49">
-        <v>627322.1392433867</v>
+        <v>5.635330657488889</v>
       </c>
       <c r="K49">
-        <v>6882912.21817465</v>
+        <v>52.64117283118716</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -3477,10 +3477,10 @@
         <v>364</v>
       </c>
       <c r="J50">
-        <v>627125.3170264955</v>
+        <v>5.633562573432012</v>
       </c>
       <c r="K50">
-        <v>6882585.620353284</v>
+        <v>52.63938808530209</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -3512,10 +3512,10 @@
         <v>364</v>
       </c>
       <c r="J51">
-        <v>627125.3170264955</v>
+        <v>5.633562573432012</v>
       </c>
       <c r="K51">
-        <v>6882585.620353284</v>
+        <v>52.63938808530209</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -3547,10 +3547,10 @@
         <v>364</v>
       </c>
       <c r="J52">
-        <v>627125.3170264955</v>
+        <v>5.633562573432012</v>
       </c>
       <c r="K52">
-        <v>6882585.620353284</v>
+        <v>52.63938808530209</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -3582,10 +3582,10 @@
         <v>365</v>
       </c>
       <c r="J53">
-        <v>639798.0298312898</v>
+        <v>5.747403489470051</v>
       </c>
       <c r="K53">
-        <v>6902698.396361711</v>
+        <v>52.74916109401226</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -3617,10 +3617,10 @@
         <v>365</v>
       </c>
       <c r="J54">
-        <v>639798.0298312898</v>
+        <v>5.747403489470051</v>
       </c>
       <c r="K54">
-        <v>6902698.396361711</v>
+        <v>52.74916109401226</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -3652,10 +3652,10 @@
         <v>366</v>
       </c>
       <c r="J55">
-        <v>639814.5161055208</v>
+        <v>5.747551588191251</v>
       </c>
       <c r="K55">
-        <v>6902698.314131074</v>
+        <v>52.74916064577468</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -3687,10 +3687,10 @@
         <v>366</v>
       </c>
       <c r="J56">
-        <v>639814.5161055208</v>
+        <v>5.747551588191251</v>
       </c>
       <c r="K56">
-        <v>6902698.314131074</v>
+        <v>52.74916064577468</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -3722,10 +3722,10 @@
         <v>367</v>
       </c>
       <c r="J57">
-        <v>623622.7808753886</v>
+        <v>5.602098755854809</v>
       </c>
       <c r="K57">
-        <v>6844055.484563485</v>
+        <v>52.42832007351137</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -3757,10 +3757,10 @@
         <v>367</v>
       </c>
       <c r="J58">
-        <v>623622.7808753886</v>
+        <v>5.602098755854809</v>
       </c>
       <c r="K58">
-        <v>6844055.484563485</v>
+        <v>52.42832007351137</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -3792,10 +3792,10 @@
         <v>368</v>
       </c>
       <c r="J59">
-        <v>622533.6980640789</v>
+        <v>5.592315358504094</v>
       </c>
       <c r="K59">
-        <v>6845548.17729116</v>
+        <v>52.43651603250899</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -3827,10 +3827,10 @@
         <v>369</v>
       </c>
       <c r="J60">
-        <v>639557.0575374895</v>
+        <v>5.745238798524349</v>
       </c>
       <c r="K60">
-        <v>6871422.563169483</v>
+        <v>52.57834177200539</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -3862,10 +3862,10 @@
         <v>369</v>
       </c>
       <c r="J61">
-        <v>639557.0575374895</v>
+        <v>5.745238798524349</v>
       </c>
       <c r="K61">
-        <v>6871422.563169483</v>
+        <v>52.57834177200539</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -3897,10 +3897,10 @@
         <v>370</v>
       </c>
       <c r="J62">
-        <v>639422.5239744168</v>
+        <v>5.744030262964997</v>
       </c>
       <c r="K62">
-        <v>6871449.504573588</v>
+        <v>52.57848920677466</v>
       </c>
     </row>
     <row r="63" spans="1:11">
@@ -3932,10 +3932,10 @@
         <v>370</v>
       </c>
       <c r="J63">
-        <v>639422.5239744168</v>
+        <v>5.744030262964997</v>
       </c>
       <c r="K63">
-        <v>6871449.504573588</v>
+        <v>52.57848920677466</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -3967,10 +3967,10 @@
         <v>370</v>
       </c>
       <c r="J64">
-        <v>639422.5239744168</v>
+        <v>5.744030262964997</v>
       </c>
       <c r="K64">
-        <v>6871449.504573588</v>
+        <v>52.57848920677466</v>
       </c>
     </row>
     <row r="65" spans="1:11">
@@ -4002,10 +4002,10 @@
         <v>371</v>
       </c>
       <c r="J65">
-        <v>629858.6037864573</v>
+        <v>5.658116106155565</v>
       </c>
       <c r="K65">
-        <v>6847117.042654197</v>
+        <v>52.44512858320331</v>
       </c>
     </row>
     <row r="66" spans="1:11">
@@ -4037,10 +4037,10 @@
         <v>371</v>
       </c>
       <c r="J66">
-        <v>629858.6037864573</v>
+        <v>5.658116106155565</v>
       </c>
       <c r="K66">
-        <v>6847117.042654197</v>
+        <v>52.44512858320331</v>
       </c>
     </row>
     <row r="67" spans="1:11">
@@ -4072,10 +4072,10 @@
         <v>372</v>
       </c>
       <c r="J67">
-        <v>629887.9156513029</v>
+        <v>5.658379419117534</v>
       </c>
       <c r="K67">
-        <v>6847074.362616817</v>
+        <v>52.44489430633676</v>
       </c>
     </row>
     <row r="68" spans="1:11">
@@ -4107,10 +4107,10 @@
         <v>372</v>
       </c>
       <c r="J68">
-        <v>629887.9156513029</v>
+        <v>5.658379419117534</v>
       </c>
       <c r="K68">
-        <v>6847074.362616817</v>
+        <v>52.44489430633676</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -4142,10 +4142,10 @@
         <v>373</v>
       </c>
       <c r="J69">
-        <v>624811.4590703091</v>
+        <v>5.612776833758774</v>
       </c>
       <c r="K69">
-        <v>6843145.187948278</v>
+        <v>52.4233211370272</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -4177,10 +4177,10 @@
         <v>373</v>
       </c>
       <c r="J70">
-        <v>624811.4590703091</v>
+        <v>5.612776833758774</v>
       </c>
       <c r="K70">
-        <v>6843145.187948278</v>
+        <v>52.4233211370272</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -4212,10 +4212,10 @@
         <v>374</v>
       </c>
       <c r="J71">
-        <v>624813.0955672998</v>
+        <v>5.612791534661365</v>
       </c>
       <c r="K71">
-        <v>6843145.182847288</v>
+        <v>52.42332110901328</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -4247,10 +4247,10 @@
         <v>374</v>
       </c>
       <c r="J72">
-        <v>624813.0955672998</v>
+        <v>5.612791534661365</v>
       </c>
       <c r="K72">
-        <v>6843145.182847288</v>
+        <v>52.42332110901328</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -4282,10 +4282,10 @@
         <v>374</v>
       </c>
       <c r="J73">
-        <v>624813.0955672998</v>
+        <v>5.612791534661365</v>
       </c>
       <c r="K73">
-        <v>6843145.182847288</v>
+        <v>52.42332110901328</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -4317,10 +4317,10 @@
         <v>375</v>
       </c>
       <c r="J74">
-        <v>619027.4140972253</v>
+        <v>5.560817873725216</v>
       </c>
       <c r="K74">
-        <v>6843571.916948595</v>
+        <v>52.42566461024887</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -4352,10 +4352,10 @@
         <v>375</v>
       </c>
       <c r="J75">
-        <v>619027.4140972253</v>
+        <v>5.560817873725216</v>
       </c>
       <c r="K75">
-        <v>6843571.916948595</v>
+        <v>52.42566461024887</v>
       </c>
     </row>
     <row r="76" spans="1:11">
@@ -4387,10 +4387,10 @@
         <v>376</v>
       </c>
       <c r="J76">
-        <v>618998.8226262622</v>
+        <v>5.560561032171599</v>
       </c>
       <c r="K76">
-        <v>6841884.830314618</v>
+        <v>52.41639888357573</v>
       </c>
     </row>
     <row r="77" spans="1:11">
@@ -4422,10 +4422,10 @@
         <v>376</v>
       </c>
       <c r="J77">
-        <v>618998.8226262622</v>
+        <v>5.560561032171599</v>
       </c>
       <c r="K77">
-        <v>6841884.830314618</v>
+        <v>52.41639888357573</v>
       </c>
     </row>
     <row r="78" spans="1:11">
@@ -4457,10 +4457,10 @@
         <v>376</v>
       </c>
       <c r="J78">
-        <v>618998.8226262622</v>
+        <v>5.560561032171599</v>
       </c>
       <c r="K78">
-        <v>6841884.830314618</v>
+        <v>52.41639888357573</v>
       </c>
     </row>
     <row r="79" spans="1:11">
@@ -4492,10 +4492,10 @@
         <v>377</v>
       </c>
       <c r="J79">
-        <v>627750.3559306372</v>
+        <v>5.639177393439611</v>
       </c>
       <c r="K79">
-        <v>6848706.467726416</v>
+        <v>52.45385227456811</v>
       </c>
     </row>
     <row r="80" spans="1:11">
@@ -4527,10 +4527,10 @@
         <v>377</v>
       </c>
       <c r="J80">
-        <v>627750.3559306372</v>
+        <v>5.639177393439611</v>
       </c>
       <c r="K80">
-        <v>6848706.467726416</v>
+        <v>52.45385227456811</v>
       </c>
     </row>
     <row r="81" spans="1:11">
@@ -4562,10 +4562,10 @@
         <v>378</v>
       </c>
       <c r="J81">
-        <v>627738.921064858</v>
+        <v>5.639074672292598</v>
       </c>
       <c r="K81">
-        <v>6848714.695758773</v>
+        <v>52.45389743028845</v>
       </c>
     </row>
     <row r="82" spans="1:11">
@@ -4597,10 +4597,10 @@
         <v>378</v>
       </c>
       <c r="J82">
-        <v>627738.921064858</v>
+        <v>5.639074672292598</v>
       </c>
       <c r="K82">
-        <v>6848714.695758773</v>
+        <v>52.45389743028845</v>
       </c>
     </row>
     <row r="83" spans="1:11">
@@ -4632,10 +4632,10 @@
         <v>379</v>
       </c>
       <c r="J83">
-        <v>637329.1604652201</v>
+        <v>5.725225258609703</v>
       </c>
       <c r="K83">
-        <v>6855415.689658398</v>
+        <v>52.49065726287612</v>
       </c>
     </row>
     <row r="84" spans="1:11">
@@ -4667,10 +4667,10 @@
         <v>379</v>
       </c>
       <c r="J84">
-        <v>637329.1604652201</v>
+        <v>5.725225258609703</v>
       </c>
       <c r="K84">
-        <v>6855415.689658398</v>
+        <v>52.49065726287612</v>
       </c>
     </row>
     <row r="85" spans="1:11">
@@ -4702,10 +4702,10 @@
         <v>379</v>
       </c>
       <c r="J85">
-        <v>637329.1604652201</v>
+        <v>5.725225258609703</v>
       </c>
       <c r="K85">
-        <v>6855415.689658398</v>
+        <v>52.49065726287612</v>
       </c>
     </row>
     <row r="86" spans="1:11">
@@ -4737,10 +4737,10 @@
         <v>380</v>
       </c>
       <c r="J86">
-        <v>637329.16812207</v>
+        <v>5.725225327392356</v>
       </c>
       <c r="K86">
-        <v>6855417.328635846</v>
+        <v>52.49066625008681</v>
       </c>
     </row>
     <row r="87" spans="1:11">
@@ -4772,10 +4772,10 @@
         <v>380</v>
       </c>
       <c r="J87">
-        <v>637329.16812207</v>
+        <v>5.725225327392356</v>
       </c>
       <c r="K87">
-        <v>6855417.328635846</v>
+        <v>52.49066625008681</v>
       </c>
     </row>
     <row r="88" spans="1:11">
@@ -4807,10 +4807,10 @@
         <v>381</v>
       </c>
       <c r="J88">
-        <v>624443.40485739</v>
+        <v>5.609470546510277</v>
       </c>
       <c r="K88">
-        <v>6858660.661509362</v>
+        <v>52.50844720874757</v>
       </c>
     </row>
     <row r="89" spans="1:11">
@@ -4842,10 +4842,10 @@
         <v>381</v>
       </c>
       <c r="J89">
-        <v>624443.40485739</v>
+        <v>5.609470546510277</v>
       </c>
       <c r="K89">
-        <v>6858660.661509362</v>
+        <v>52.50844720874757</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -4877,10 +4877,10 @@
         <v>382</v>
       </c>
       <c r="J90">
-        <v>626182.8894762024</v>
+        <v>5.625096602705977</v>
       </c>
       <c r="K90">
-        <v>6858599.379804738</v>
+        <v>52.50811131038396</v>
       </c>
     </row>
     <row r="91" spans="1:11">
@@ -4912,10 +4912,10 @@
         <v>382</v>
       </c>
       <c r="J91">
-        <v>626182.8894762024</v>
+        <v>5.625096602705977</v>
       </c>
       <c r="K91">
-        <v>6858599.379804738</v>
+        <v>52.50811131038396</v>
       </c>
     </row>
     <row r="92" spans="1:11">
@@ -4947,10 +4947,10 @@
         <v>382</v>
       </c>
       <c r="J92">
-        <v>626182.8894762024</v>
+        <v>5.625096602705977</v>
       </c>
       <c r="K92">
-        <v>6858599.379804738</v>
+        <v>52.50811131038396</v>
       </c>
     </row>
     <row r="93" spans="1:11">
@@ -4982,10 +4982,10 @@
         <v>383</v>
       </c>
       <c r="J93">
-        <v>632015.1153749432</v>
+        <v>5.677488379358743</v>
       </c>
       <c r="K93">
-        <v>6859817.760467649</v>
+        <v>52.51478903579811</v>
       </c>
     </row>
     <row r="94" spans="1:11">
@@ -5017,10 +5017,10 @@
         <v>383</v>
       </c>
       <c r="J94">
-        <v>632015.1153749432</v>
+        <v>5.677488379358743</v>
       </c>
       <c r="K94">
-        <v>6859817.760467649</v>
+        <v>52.51478903579811</v>
       </c>
     </row>
     <row r="95" spans="1:11">
@@ -5052,10 +5052,10 @@
         <v>384</v>
       </c>
       <c r="J95">
-        <v>631838.0280555513</v>
+        <v>5.675897576902408</v>
       </c>
       <c r="K95">
-        <v>6859823.388878135</v>
+        <v>52.51481988173804</v>
       </c>
     </row>
     <row r="96" spans="1:11">
@@ -5087,10 +5087,10 @@
         <v>384</v>
       </c>
       <c r="J96">
-        <v>631838.0280555513</v>
+        <v>5.675897576902408</v>
       </c>
       <c r="K96">
-        <v>6859823.388878135</v>
+        <v>52.51481988173804</v>
       </c>
     </row>
     <row r="97" spans="1:11">
@@ -5122,10 +5122,10 @@
         <v>385</v>
       </c>
       <c r="J97">
-        <v>612149.8555157806</v>
+        <v>5.499035713813825</v>
       </c>
       <c r="K97">
-        <v>6850606.275022324</v>
+        <v>52.4642772463945</v>
       </c>
     </row>
     <row r="98" spans="1:11">
@@ -5157,10 +5157,10 @@
         <v>385</v>
       </c>
       <c r="J98">
-        <v>612149.8555157806</v>
+        <v>5.499035713813825</v>
       </c>
       <c r="K98">
-        <v>6850606.275022324</v>
+        <v>52.4642772463945</v>
       </c>
     </row>
     <row r="99" spans="1:11">
@@ -5192,10 +5192,10 @@
         <v>386</v>
       </c>
       <c r="J99">
-        <v>612149.8301782944</v>
+        <v>5.499035486203314</v>
       </c>
       <c r="K99">
-        <v>6850589.894837412</v>
+        <v>52.46418737263453</v>
       </c>
     </row>
     <row r="100" spans="1:11">
@@ -5227,10 +5227,10 @@
         <v>386</v>
       </c>
       <c r="J100">
-        <v>612149.8301782944</v>
+        <v>5.499035486203314</v>
       </c>
       <c r="K100">
-        <v>6850589.894837412</v>
+        <v>52.46418737263453</v>
       </c>
     </row>
     <row r="101" spans="1:11">
@@ -5262,10 +5262,10 @@
         <v>386</v>
       </c>
       <c r="J101">
-        <v>612149.8301782944</v>
+        <v>5.499035486203314</v>
       </c>
       <c r="K101">
-        <v>6850589.894837412</v>
+        <v>52.46418737263453</v>
       </c>
     </row>
     <row r="102" spans="1:11">
@@ -5297,10 +5297,10 @@
         <v>387</v>
       </c>
       <c r="J102">
-        <v>615154.3498754905</v>
+        <v>5.526025545857608</v>
       </c>
       <c r="K102">
-        <v>6847379.718630455</v>
+        <v>52.44657042186665</v>
       </c>
     </row>
     <row r="103" spans="1:11">
@@ -5332,10 +5332,10 @@
         <v>387</v>
       </c>
       <c r="J103">
-        <v>615154.3498754905</v>
+        <v>5.526025545857608</v>
       </c>
       <c r="K103">
-        <v>6847379.718630455</v>
+        <v>52.44657042186665</v>
       </c>
     </row>
     <row r="104" spans="1:11">
@@ -5367,10 +5367,10 @@
         <v>387</v>
       </c>
       <c r="J104">
-        <v>615154.3498754905</v>
+        <v>5.526025545857608</v>
       </c>
       <c r="K104">
-        <v>6847379.718630455</v>
+        <v>52.44657042186665</v>
       </c>
     </row>
     <row r="105" spans="1:11">
@@ -5402,10 +5402,10 @@
         <v>388</v>
       </c>
       <c r="J105">
-        <v>615046.5429271793</v>
+        <v>5.525057099563585</v>
       </c>
       <c r="K105">
-        <v>6847515.827626682</v>
+        <v>52.44731751079249</v>
       </c>
     </row>
     <row r="106" spans="1:11">
@@ -5437,10 +5437,10 @@
         <v>388</v>
       </c>
       <c r="J106">
-        <v>615046.5429271793</v>
+        <v>5.525057099563585</v>
       </c>
       <c r="K106">
-        <v>6847515.827626682</v>
+        <v>52.44731751079249</v>
       </c>
     </row>
     <row r="107" spans="1:11">
@@ -5472,10 +5472,10 @@
         <v>389</v>
       </c>
       <c r="J107">
-        <v>608660.4861916584</v>
+        <v>5.467690175855856</v>
       </c>
       <c r="K107">
-        <v>6853207.604057717</v>
+        <v>52.47854771373215</v>
       </c>
     </row>
     <row r="108" spans="1:11">
@@ -5507,10 +5507,10 @@
         <v>389</v>
       </c>
       <c r="J108">
-        <v>608660.4861916584</v>
+        <v>5.467690175855856</v>
       </c>
       <c r="K108">
-        <v>6853207.604057717</v>
+        <v>52.47854771373215</v>
       </c>
     </row>
     <row r="109" spans="1:11">
@@ -5542,10 +5542,10 @@
         <v>390</v>
       </c>
       <c r="J109">
-        <v>608660.467937963</v>
+        <v>5.467690011880121</v>
       </c>
       <c r="K109">
-        <v>6853191.218572761</v>
+        <v>52.47845784018428</v>
       </c>
     </row>
     <row r="110" spans="1:11">
@@ -5577,10 +5577,10 @@
         <v>390</v>
       </c>
       <c r="J110">
-        <v>608660.467937963</v>
+        <v>5.467690011880121</v>
       </c>
       <c r="K110">
-        <v>6853191.218572761</v>
+        <v>52.47845784018428</v>
       </c>
     </row>
     <row r="111" spans="1:11">
@@ -5612,10 +5612,10 @@
         <v>390</v>
       </c>
       <c r="J111">
-        <v>608660.467937963</v>
+        <v>5.467690011880121</v>
       </c>
       <c r="K111">
-        <v>6853191.218572761</v>
+        <v>52.47845784018428</v>
       </c>
     </row>
     <row r="112" spans="1:11">
@@ -5647,10 +5647,10 @@
         <v>391</v>
       </c>
       <c r="J112">
-        <v>607868.7118403557</v>
+        <v>5.460577545842366</v>
       </c>
       <c r="K112">
-        <v>6852859.443142777</v>
+        <v>52.47663802921268</v>
       </c>
     </row>
     <row r="113" spans="1:11">
@@ -5682,10 +5682,10 @@
         <v>391</v>
       </c>
       <c r="J113">
-        <v>607868.7118403557</v>
+        <v>5.460577545842366</v>
       </c>
       <c r="K113">
-        <v>6852859.443142777</v>
+        <v>52.47663802921268</v>
       </c>
     </row>
     <row r="114" spans="1:11">
@@ -5717,10 +5717,10 @@
         <v>392</v>
       </c>
       <c r="J114">
-        <v>607867.0733607284</v>
+        <v>5.460562827129448</v>
       </c>
       <c r="K114">
-        <v>6852859.444806904</v>
+        <v>52.47663803834072</v>
       </c>
     </row>
     <row r="115" spans="1:11">
@@ -5752,10 +5752,10 @@
         <v>392</v>
       </c>
       <c r="J115">
-        <v>607867.0733607284</v>
+        <v>5.460562827129448</v>
       </c>
       <c r="K115">
-        <v>6852859.444806904</v>
+        <v>52.47663803834072</v>
       </c>
     </row>
     <row r="116" spans="1:11">
@@ -5787,10 +5787,10 @@
         <v>393</v>
       </c>
       <c r="J116">
-        <v>638862.7106414264</v>
+        <v>5.739001374232205</v>
       </c>
       <c r="K116">
-        <v>6858670.674769487</v>
+        <v>52.5085020933609</v>
       </c>
     </row>
     <row r="117" spans="1:11">
@@ -5822,10 +5822,10 @@
         <v>393</v>
       </c>
       <c r="J117">
-        <v>638862.7106414264</v>
+        <v>5.739001374232205</v>
       </c>
       <c r="K117">
-        <v>6858670.674769487</v>
+        <v>52.5085020933609</v>
       </c>
     </row>
     <row r="118" spans="1:11">
@@ -5857,10 +5857,10 @@
         <v>394</v>
       </c>
       <c r="J118">
-        <v>638700.3865048984</v>
+        <v>5.73754319170396</v>
       </c>
       <c r="K118">
-        <v>6858671.462454493</v>
+        <v>52.50850641081168</v>
       </c>
     </row>
     <row r="119" spans="1:11">
@@ -5892,10 +5892,10 @@
         <v>394</v>
       </c>
       <c r="J119">
-        <v>638700.3865048984</v>
+        <v>5.73754319170396</v>
       </c>
       <c r="K119">
-        <v>6858671.462454493</v>
+        <v>52.50850641081168</v>
       </c>
     </row>
     <row r="120" spans="1:11">
@@ -5927,10 +5927,10 @@
         <v>395</v>
       </c>
       <c r="J120">
-        <v>632198.5002912073</v>
+        <v>5.679135754090312</v>
       </c>
       <c r="K120">
-        <v>6842693.297169053</v>
+        <v>52.42083934604499</v>
       </c>
     </row>
     <row r="121" spans="1:11">
@@ -5962,10 +5962,10 @@
         <v>395</v>
       </c>
       <c r="J121">
-        <v>632198.5002912073</v>
+        <v>5.679135754090312</v>
       </c>
       <c r="K121">
-        <v>6842693.297169053</v>
+        <v>52.42083934604499</v>
       </c>
     </row>
     <row r="122" spans="1:11">
@@ -5997,10 +5997,10 @@
         <v>396</v>
       </c>
       <c r="J122">
-        <v>632196.8638929026</v>
+        <v>5.679121054074233</v>
       </c>
       <c r="K122">
-        <v>6842693.303768688</v>
+        <v>52.42083938229131</v>
       </c>
     </row>
     <row r="123" spans="1:11">
@@ -6032,10 +6032,10 @@
         <v>396</v>
       </c>
       <c r="J123">
-        <v>632196.8638929026</v>
+        <v>5.679121054074233</v>
       </c>
       <c r="K123">
-        <v>6842693.303768688</v>
+        <v>52.42083938229131</v>
       </c>
     </row>
     <row r="124" spans="1:11">
@@ -6067,10 +6067,10 @@
         <v>397</v>
       </c>
       <c r="J124">
-        <v>564591.5888895027</v>
+        <v>5.071812535847656</v>
       </c>
       <c r="K124">
-        <v>6918490.371498683</v>
+        <v>52.83515740671481</v>
       </c>
     </row>
     <row r="125" spans="1:11">
@@ -6102,10 +6102,10 @@
         <v>397</v>
       </c>
       <c r="J125">
-        <v>564591.5888895027</v>
+        <v>5.071812535847656</v>
       </c>
       <c r="K125">
-        <v>6918490.371498683</v>
+        <v>52.83515740671481</v>
       </c>
     </row>
     <row r="126" spans="1:11">
@@ -6137,10 +6137,10 @@
         <v>398</v>
       </c>
       <c r="J126">
-        <v>562939.7315095988</v>
+        <v>5.056973648532123</v>
       </c>
       <c r="K126">
-        <v>6918479.688106614</v>
+        <v>52.83509928728925</v>
       </c>
     </row>
     <row r="127" spans="1:11">
@@ -6172,10 +6172,10 @@
         <v>398</v>
       </c>
       <c r="J127">
-        <v>562939.7315095988</v>
+        <v>5.056973648532123</v>
       </c>
       <c r="K127">
-        <v>6918479.688106614</v>
+        <v>52.83509928728925</v>
       </c>
     </row>
     <row r="128" spans="1:11">
@@ -6207,10 +6207,10 @@
         <v>399</v>
       </c>
       <c r="J128">
-        <v>564184.7322829454</v>
+        <v>5.068157680766503</v>
       </c>
       <c r="K128">
-        <v>6917104.407710172</v>
+        <v>52.82761688114269</v>
       </c>
     </row>
     <row r="129" spans="1:11">
@@ -6242,10 +6242,10 @@
         <v>399</v>
       </c>
       <c r="J129">
-        <v>564184.7322829454</v>
+        <v>5.068157680766503</v>
       </c>
       <c r="K129">
-        <v>6917104.407710172</v>
+        <v>52.82761688114269</v>
       </c>
     </row>
     <row r="130" spans="1:11">
@@ -6277,10 +6277,10 @@
         <v>400</v>
       </c>
       <c r="J130">
-        <v>564052.1513856278</v>
+        <v>5.066966686302075</v>
       </c>
       <c r="K130">
-        <v>6917206.222421963</v>
+        <v>52.82817086277342</v>
       </c>
     </row>
     <row r="131" spans="1:11">
@@ -6312,10 +6312,10 @@
         <v>400</v>
       </c>
       <c r="J131">
-        <v>564052.1513856278</v>
+        <v>5.066966686302075</v>
       </c>
       <c r="K131">
-        <v>6917206.222421963</v>
+        <v>52.82817086277342</v>
       </c>
     </row>
     <row r="132" spans="1:11">
@@ -6347,10 +6347,10 @@
         <v>401</v>
       </c>
       <c r="J132">
-        <v>568027.1141880923</v>
+        <v>5.10267438469468</v>
       </c>
       <c r="K132">
-        <v>6908955.677622048</v>
+        <v>52.78325599507085</v>
       </c>
     </row>
     <row r="133" spans="1:11">
@@ -6382,10 +6382,10 @@
         <v>401</v>
       </c>
       <c r="J133">
-        <v>568027.1141880923</v>
+        <v>5.10267438469468</v>
       </c>
       <c r="K133">
-        <v>6908955.677622048</v>
+        <v>52.78325599507085</v>
       </c>
     </row>
     <row r="134" spans="1:11">
@@ -6417,10 +6417,10 @@
         <v>402</v>
       </c>
       <c r="J134">
-        <v>568027.0492469635</v>
+        <v>5.102673801318594</v>
       </c>
       <c r="K134">
-        <v>6908972.176843449</v>
+        <v>52.78334586116521</v>
       </c>
     </row>
     <row r="135" spans="1:11">
@@ -6452,10 +6452,10 @@
         <v>402</v>
       </c>
       <c r="J135">
-        <v>568027.0492469635</v>
+        <v>5.102673801318594</v>
       </c>
       <c r="K135">
-        <v>6908972.176843449</v>
+        <v>52.78334586116521</v>
       </c>
     </row>
     <row r="136" spans="1:11">
@@ -6487,10 +6487,10 @@
         <v>402</v>
       </c>
       <c r="J136">
-        <v>568027.0492469635</v>
+        <v>5.102673801318594</v>
       </c>
       <c r="K136">
-        <v>6908972.176843449</v>
+        <v>52.78334586116521</v>
       </c>
     </row>
     <row r="137" spans="1:11">
@@ -6522,10 +6522,10 @@
         <v>402</v>
       </c>
       <c r="J137">
-        <v>568027.0492469635</v>
+        <v>5.102673801318594</v>
       </c>
       <c r="K137">
-        <v>6908972.176843449</v>
+        <v>52.78334586116521</v>
       </c>
     </row>
     <row r="138" spans="1:11">
@@ -6557,10 +6557,10 @@
         <v>403</v>
       </c>
       <c r="J138">
-        <v>558215.3713765166</v>
+        <v>5.014533999379798</v>
       </c>
       <c r="K138">
-        <v>6921344.754190781</v>
+        <v>52.85068292250649</v>
       </c>
     </row>
     <row r="139" spans="1:11">
@@ -6592,10 +6592,10 @@
         <v>403</v>
       </c>
       <c r="J139">
-        <v>558215.3713765166</v>
+        <v>5.014533999379798</v>
       </c>
       <c r="K139">
-        <v>6921344.754190781</v>
+        <v>52.85068292250649</v>
       </c>
     </row>
     <row r="140" spans="1:11">
@@ -6627,10 +6627,10 @@
         <v>404</v>
       </c>
       <c r="J140">
-        <v>558215.3799004626</v>
+        <v>5.014534075951707</v>
       </c>
       <c r="K140">
-        <v>6921343.101738252</v>
+        <v>52.85067393612504</v>
       </c>
     </row>
     <row r="141" spans="1:11">
@@ -6662,10 +6662,10 @@
         <v>404</v>
       </c>
       <c r="J141">
-        <v>558215.3799004626</v>
+        <v>5.014534075951707</v>
       </c>
       <c r="K141">
-        <v>6921343.101738252</v>
+        <v>52.85067393612504</v>
       </c>
     </row>
     <row r="142" spans="1:11">
@@ -6697,10 +6697,10 @@
         <v>405</v>
       </c>
       <c r="J142">
-        <v>561800.3181996377</v>
+        <v>5.046738124619451</v>
       </c>
       <c r="K142">
-        <v>6915940.778253664</v>
+        <v>52.82128498012977</v>
       </c>
     </row>
     <row r="143" spans="1:11">
@@ -6732,10 +6732,10 @@
         <v>405</v>
       </c>
       <c r="J143">
-        <v>561800.3181996377</v>
+        <v>5.046738124619451</v>
       </c>
       <c r="K143">
-        <v>6915940.778253664</v>
+        <v>52.82128498012977</v>
       </c>
     </row>
     <row r="144" spans="1:11">
@@ -6767,10 +6767,10 @@
         <v>405</v>
       </c>
       <c r="J144">
-        <v>561800.3181996377</v>
+        <v>5.046738124619451</v>
       </c>
       <c r="K144">
-        <v>6915940.778253664</v>
+        <v>52.82128498012977</v>
       </c>
     </row>
     <row r="145" spans="1:11">
@@ -6802,10 +6802,10 @@
         <v>406</v>
       </c>
       <c r="J145">
-        <v>561801.0962074423</v>
+        <v>5.046745113582472</v>
       </c>
       <c r="K145">
-        <v>6915775.645242449</v>
+        <v>52.8203863321109</v>
       </c>
     </row>
     <row r="146" spans="1:11">
@@ -6837,10 +6837,10 @@
         <v>406</v>
       </c>
       <c r="J146">
-        <v>561801.0962074423</v>
+        <v>5.046745113582472</v>
       </c>
       <c r="K146">
-        <v>6915775.645242449</v>
+        <v>52.8203863321109</v>
       </c>
     </row>
     <row r="147" spans="1:11">
@@ -6872,10 +6872,10 @@
         <v>406</v>
       </c>
       <c r="J147">
-        <v>561801.0962074423</v>
+        <v>5.046745113582472</v>
       </c>
       <c r="K147">
-        <v>6915775.645242449</v>
+        <v>52.8203863321109</v>
       </c>
     </row>
     <row r="148" spans="1:11">
@@ -6907,10 +6907,10 @@
         <v>407</v>
       </c>
       <c r="J148">
-        <v>550894.2548993153</v>
+        <v>4.948767291096905</v>
       </c>
       <c r="K148">
-        <v>6907012.374623039</v>
+        <v>52.77267012731232</v>
       </c>
     </row>
     <row r="149" spans="1:11">
@@ -6942,10 +6942,10 @@
         <v>407</v>
       </c>
       <c r="J149">
-        <v>550894.2548993153</v>
+        <v>4.948767291096905</v>
       </c>
       <c r="K149">
-        <v>6907012.374623039</v>
+        <v>52.77267012731232</v>
       </c>
     </row>
     <row r="150" spans="1:11">
@@ -6977,10 +6977,10 @@
         <v>408</v>
       </c>
       <c r="J150">
-        <v>552541.6501455882</v>
+        <v>4.963566094384033</v>
       </c>
       <c r="K150">
-        <v>6906537.24272937</v>
+        <v>52.77008151999907</v>
       </c>
     </row>
     <row r="151" spans="1:11">
@@ -7012,10 +7012,10 @@
         <v>408</v>
       </c>
       <c r="J151">
-        <v>552541.6501455882</v>
+        <v>4.963566094384033</v>
       </c>
       <c r="K151">
-        <v>6906537.24272937</v>
+        <v>52.77008151999907</v>
       </c>
     </row>
     <row r="152" spans="1:11">
@@ -7047,10 +7047,10 @@
         <v>409</v>
       </c>
       <c r="J152">
-        <v>563630.5226015913</v>
+        <v>5.063179130492828</v>
       </c>
       <c r="K152">
-        <v>6908103.991852495</v>
+        <v>52.77861687599245</v>
       </c>
     </row>
     <row r="153" spans="1:11">
@@ -7082,10 +7082,10 @@
         <v>409</v>
       </c>
       <c r="J153">
-        <v>563630.5226015913</v>
+        <v>5.063179130492828</v>
       </c>
       <c r="K153">
-        <v>6908103.991852495</v>
+        <v>52.77861687599245</v>
       </c>
     </row>
     <row r="154" spans="1:11">
@@ -7117,10 +7117,10 @@
         <v>410</v>
       </c>
       <c r="J154">
-        <v>563526.0252824926</v>
+        <v>5.06224041510387</v>
       </c>
       <c r="K154">
-        <v>6908228.9065566</v>
+        <v>52.77929731553227</v>
       </c>
     </row>
     <row r="155" spans="1:11">
@@ -7152,10 +7152,10 @@
         <v>410</v>
       </c>
       <c r="J155">
-        <v>563526.0252824926</v>
+        <v>5.06224041510387</v>
       </c>
       <c r="K155">
-        <v>6908228.9065566</v>
+        <v>52.77929731553227</v>
       </c>
     </row>
     <row r="156" spans="1:11">
@@ -7187,10 +7187,10 @@
         <v>411</v>
       </c>
       <c r="J156">
-        <v>561658.5046929332</v>
+        <v>5.045464192213778</v>
       </c>
       <c r="K156">
-        <v>6916595.734906507</v>
+        <v>52.82484904720382</v>
       </c>
     </row>
     <row r="157" spans="1:11">
@@ -7222,10 +7222,10 @@
         <v>411</v>
       </c>
       <c r="J157">
-        <v>561658.5046929332</v>
+        <v>5.045464192213778</v>
       </c>
       <c r="K157">
-        <v>6916595.734906507</v>
+        <v>52.82484904720382</v>
       </c>
     </row>
     <row r="158" spans="1:11">
@@ -7257,10 +7257,10 @@
         <v>411</v>
       </c>
       <c r="J158">
-        <v>561658.5046929332</v>
+        <v>5.045464192213778</v>
       </c>
       <c r="K158">
-        <v>6916595.734906507</v>
+        <v>52.82484904720382</v>
       </c>
     </row>
     <row r="159" spans="1:11">
@@ -7292,10 +7292,10 @@
         <v>412</v>
       </c>
       <c r="J159">
-        <v>561656.923506299</v>
+        <v>5.045449988172574</v>
       </c>
       <c r="K159">
-        <v>6916580.863777193</v>
+        <v>52.82476812647808</v>
       </c>
     </row>
     <row r="160" spans="1:11">
@@ -7327,10 +7327,10 @@
         <v>412</v>
       </c>
       <c r="J160">
-        <v>561656.923506299</v>
+        <v>5.045449988172574</v>
       </c>
       <c r="K160">
-        <v>6916580.863777193</v>
+        <v>52.82476812647808</v>
       </c>
     </row>
     <row r="161" spans="1:11">
@@ -7362,10 +7362,10 @@
         <v>413</v>
       </c>
       <c r="J161">
-        <v>565987.1137058334</v>
+        <v>5.084348748566437</v>
       </c>
       <c r="K161">
-        <v>6925667.158879593</v>
+        <v>52.87418266324956</v>
       </c>
     </row>
     <row r="162" spans="1:11">
@@ -7397,10 +7397,10 @@
         <v>413</v>
       </c>
       <c r="J162">
-        <v>565987.1137058334</v>
+        <v>5.084348748566437</v>
       </c>
       <c r="K162">
-        <v>6925667.158879593</v>
+        <v>52.87418266324956</v>
       </c>
     </row>
     <row r="163" spans="1:11">
@@ -7432,10 +7432,10 @@
         <v>413</v>
       </c>
       <c r="J163">
-        <v>565987.1137058334</v>
+        <v>5.084348748566437</v>
       </c>
       <c r="K163">
-        <v>6925667.158879593</v>
+        <v>52.87418266324956</v>
       </c>
     </row>
     <row r="164" spans="1:11">
@@ -7467,10 +7467,10 @@
         <v>414</v>
       </c>
       <c r="J164">
-        <v>565988.7670570472</v>
+        <v>5.084363600873091</v>
       </c>
       <c r="K164">
-        <v>6925667.165810666</v>
+        <v>52.87418270092166</v>
       </c>
     </row>
     <row r="165" spans="1:11">
@@ -7502,10 +7502,10 @@
         <v>414</v>
       </c>
       <c r="J165">
-        <v>565988.7670570472</v>
+        <v>5.084363600873091</v>
       </c>
       <c r="K165">
-        <v>6925667.165810666</v>
+        <v>52.87418270092166</v>
       </c>
     </row>
     <row r="166" spans="1:11">
@@ -7537,10 +7537,10 @@
         <v>415</v>
       </c>
       <c r="J166">
-        <v>567783.7039193974</v>
+        <v>5.100487793047877</v>
       </c>
       <c r="K166">
-        <v>6917913.961476444</v>
+        <v>52.83202152890757</v>
       </c>
     </row>
     <row r="167" spans="1:11">
@@ -7572,10 +7572,10 @@
         <v>415</v>
       </c>
       <c r="J167">
-        <v>567783.7039193974</v>
+        <v>5.100487793047877</v>
       </c>
       <c r="K167">
-        <v>6917913.961476444</v>
+        <v>52.83202152890757</v>
       </c>
     </row>
     <row r="168" spans="1:11">
@@ -7607,10 +7607,10 @@
         <v>416</v>
       </c>
       <c r="J168">
-        <v>566171.4029992243</v>
+        <v>5.086004247455962</v>
       </c>
       <c r="K168">
-        <v>6917555.5803947</v>
+        <v>52.83007169224504</v>
       </c>
     </row>
     <row r="169" spans="1:11">
@@ -7642,10 +7642,10 @@
         <v>416</v>
       </c>
       <c r="J169">
-        <v>566171.4029992243</v>
+        <v>5.086004247455962</v>
       </c>
       <c r="K169">
-        <v>6917555.5803947</v>
+        <v>52.83007169224504</v>
       </c>
     </row>
     <row r="170" spans="1:11">
@@ -7677,10 +7677,10 @@
         <v>417</v>
       </c>
       <c r="J170">
-        <v>565019.5471161997</v>
+        <v>5.075656950007723</v>
       </c>
       <c r="K170">
-        <v>6922295.814725481</v>
+        <v>52.85585467786636</v>
       </c>
     </row>
     <row r="171" spans="1:11">
@@ -7712,10 +7712,10 @@
         <v>417</v>
       </c>
       <c r="J171">
-        <v>565019.5471161997</v>
+        <v>5.075656950007723</v>
       </c>
       <c r="K171">
-        <v>6922295.814725481</v>
+        <v>52.85585467786636</v>
       </c>
     </row>
     <row r="172" spans="1:11">
@@ -7747,10 +7747,10 @@
         <v>418</v>
       </c>
       <c r="J172">
-        <v>565016.1919129657</v>
+        <v>5.075626809704259</v>
       </c>
       <c r="K172">
-        <v>6922307.369077818</v>
+        <v>52.85591750526866</v>
       </c>
     </row>
     <row r="173" spans="1:11">
@@ -7782,10 +7782,10 @@
         <v>418</v>
       </c>
       <c r="J173">
-        <v>565016.1919129657</v>
+        <v>5.075626809704259</v>
       </c>
       <c r="K173">
-        <v>6922307.369077818</v>
+        <v>52.85591750526866</v>
       </c>
     </row>
     <row r="174" spans="1:11">
@@ -7817,10 +7817,10 @@
         <v>419</v>
       </c>
       <c r="J174">
-        <v>557976.9263298567</v>
+        <v>5.012392011081426</v>
       </c>
       <c r="K174">
-        <v>6907750.013986221</v>
+        <v>52.77668861789061</v>
       </c>
     </row>
     <row r="175" spans="1:11">
@@ -7852,10 +7852,10 @@
         <v>419</v>
       </c>
       <c r="J175">
-        <v>557976.9263298567</v>
+        <v>5.012392011081426</v>
       </c>
       <c r="K175">
-        <v>6907750.013986221</v>
+        <v>52.77668861789061</v>
       </c>
     </row>
     <row r="176" spans="1:11">
@@ -7887,10 +7887,10 @@
         <v>419</v>
       </c>
       <c r="J176">
-        <v>557976.9263298567</v>
+        <v>5.012392011081426</v>
       </c>
       <c r="K176">
-        <v>6907750.013986221</v>
+        <v>52.77668861789061</v>
       </c>
     </row>
     <row r="177" spans="1:11">
@@ -7922,10 +7922,10 @@
         <v>420</v>
       </c>
       <c r="J177">
-        <v>557976.9177756517</v>
+        <v>5.012391934237693</v>
       </c>
       <c r="K177">
-        <v>6907751.663647342</v>
+        <v>52.77669760444939</v>
       </c>
     </row>
     <row r="178" spans="1:11">
@@ -7951,10 +7951,10 @@
         <v>421</v>
       </c>
       <c r="J178">
-        <v>608327.9250805442</v>
+        <v>5.46470272856568</v>
       </c>
       <c r="K178">
-        <v>6839529.476515237</v>
+        <v>52.40345966241028</v>
       </c>
     </row>
     <row r="179" spans="1:11">
@@ -7980,10 +7980,10 @@
         <v>422</v>
       </c>
       <c r="J179">
-        <v>607092.4760638818</v>
+        <v>5.453604501221498</v>
       </c>
       <c r="K179">
-        <v>6840831.251975645</v>
+        <v>52.41061148446781</v>
       </c>
     </row>
     <row r="180" spans="1:11">
@@ -8009,10 +8009,10 @@
         <v>423</v>
       </c>
       <c r="J180">
-        <v>601854.9059225518</v>
+        <v>5.406554608125449</v>
       </c>
       <c r="K180">
-        <v>6826422.300072547</v>
+        <v>52.33138521651187</v>
       </c>
     </row>
     <row r="181" spans="1:11">
@@ -8038,10 +8038,10 @@
         <v>424</v>
       </c>
       <c r="J181">
-        <v>601309.7514469102</v>
+        <v>5.401657402148699</v>
       </c>
       <c r="K181">
-        <v>6827943.004055552</v>
+        <v>52.33975340617269</v>
       </c>
     </row>
     <row r="182" spans="1:11">
@@ -8067,10 +8067,10 @@
         <v>425</v>
       </c>
       <c r="J182">
-        <v>594010.0746288248</v>
+        <v>5.336083289600509</v>
       </c>
       <c r="K182">
-        <v>6825476.71179399</v>
+        <v>52.32618099374913</v>
       </c>
     </row>
     <row r="183" spans="1:11">
@@ -8096,10 +8096,10 @@
         <v>426</v>
       </c>
       <c r="J183">
-        <v>594510.3798322884</v>
+        <v>5.340577607710467</v>
       </c>
       <c r="K183">
-        <v>6827041.543079308</v>
+        <v>52.33479300333752</v>
       </c>
     </row>
     <row r="184" spans="1:11">
@@ -8125,10 +8125,10 @@
         <v>427</v>
       </c>
       <c r="J184">
-        <v>594030.0324088925</v>
+        <v>5.336262573389228</v>
       </c>
       <c r="K184">
-        <v>6824959.10479718</v>
+        <v>52.32333198578596</v>
       </c>
     </row>
     <row r="185" spans="1:11">
@@ -8154,10 +8154,10 @@
         <v>428</v>
       </c>
       <c r="J185">
-        <v>595534.1803312879</v>
+        <v>5.349774564071872</v>
       </c>
       <c r="K185">
-        <v>6824337.937417271</v>
+        <v>52.31991271824837</v>
       </c>
     </row>
     <row r="186" spans="1:11">
@@ -8183,10 +8183,10 @@
         <v>429</v>
       </c>
       <c r="J186">
-        <v>596825.2168961616</v>
+        <v>5.361372142857704</v>
       </c>
       <c r="K186">
-        <v>6820930.149456345</v>
+        <v>52.30114954096469</v>
       </c>
     </row>
     <row r="187" spans="1:11">
@@ -8212,10 +8212,10 @@
         <v>430</v>
       </c>
       <c r="J187">
-        <v>596986.7843912605</v>
+        <v>5.362823528360347</v>
       </c>
       <c r="K187">
-        <v>6820933.469063375</v>
+        <v>52.30116782250991</v>
       </c>
     </row>
     <row r="188" spans="1:11">
@@ -8241,10 +8241,10 @@
         <v>431</v>
       </c>
       <c r="J188">
-        <v>599588.2241068962</v>
+        <v>5.386192658933058</v>
       </c>
       <c r="K188">
-        <v>6819135.647732114</v>
+        <v>52.29126585586744</v>
       </c>
     </row>
     <row r="189" spans="1:11">
@@ -8270,10 +8270,10 @@
         <v>432</v>
       </c>
       <c r="J189">
-        <v>599770.9693192092</v>
+        <v>5.387834287106262</v>
       </c>
       <c r="K189">
-        <v>6819243.336959521</v>
+        <v>52.2918590448272</v>
       </c>
     </row>
     <row r="190" spans="1:11">
@@ -8299,10 +8299,10 @@
         <v>433</v>
       </c>
       <c r="J190">
-        <v>607978.5984596167</v>
+        <v>5.461564674138391</v>
       </c>
       <c r="K190">
-        <v>6835469.238615422</v>
+        <v>52.38114564204505</v>
       </c>
     </row>
     <row r="191" spans="1:11">
@@ -8328,10 +8328,10 @@
         <v>434</v>
       </c>
       <c r="J191">
-        <v>608074.9141276991</v>
+        <v>5.462429892505776</v>
       </c>
       <c r="K191">
-        <v>6835328.534419212</v>
+        <v>52.38037216480185</v>
       </c>
     </row>
     <row r="192" spans="1:11">
@@ -8357,10 +8357,10 @@
         <v>435</v>
       </c>
       <c r="J192">
-        <v>603116.5195819533</v>
+        <v>5.417887876454393</v>
       </c>
       <c r="K192">
-        <v>6839929.247260191</v>
+        <v>52.40565608622961</v>
       </c>
     </row>
     <row r="193" spans="1:11">
@@ -8386,10 +8386,10 @@
         <v>436</v>
       </c>
       <c r="J193">
-        <v>603208.0673500998</v>
+        <v>5.418710264047924</v>
       </c>
       <c r="K193">
-        <v>6839791.79712062</v>
+        <v>52.40490091890363</v>
       </c>
     </row>
     <row r="194" spans="1:11">
@@ -8415,10 +8415,10 @@
         <v>437</v>
       </c>
       <c r="J194">
-        <v>604793.7235195715</v>
+        <v>5.432954455771871</v>
       </c>
       <c r="K194">
-        <v>6832903.78715138</v>
+        <v>52.36704073682102</v>
       </c>
     </row>
     <row r="195" spans="1:11">
@@ -8444,10 +8444,10 @@
         <v>438</v>
       </c>
       <c r="J195">
-        <v>604805.1717946685</v>
+        <v>5.433057297376837</v>
       </c>
       <c r="K195">
-        <v>6832915.220908703</v>
+        <v>52.36710360989914</v>
       </c>
     </row>
     <row r="196" spans="1:11">
@@ -8473,10 +8473,10 @@
         <v>439</v>
       </c>
       <c r="J196">
-        <v>609936.203946678</v>
+        <v>5.479150143431424</v>
       </c>
       <c r="K196">
-        <v>6830774.409412879</v>
+        <v>52.35532993541956</v>
       </c>
     </row>
     <row r="197" spans="1:11">
@@ -8502,10 +8502,10 @@
         <v>440</v>
       </c>
       <c r="J197">
-        <v>609952.5439167006</v>
+        <v>5.479296927879559</v>
       </c>
       <c r="K197">
-        <v>6830774.388624065</v>
+        <v>52.35532982107343</v>
       </c>
     </row>
     <row r="198" spans="1:11">
@@ -8531,10 +8531,10 @@
         <v>441</v>
       </c>
       <c r="J198">
-        <v>586532.1132754266</v>
+        <v>5.268907619822382</v>
       </c>
       <c r="K198">
-        <v>6825961.14678148</v>
+        <v>52.32884724959388</v>
       </c>
     </row>
     <row r="199" spans="1:11">
@@ -8560,10 +8560,10 @@
         <v>442</v>
       </c>
       <c r="J199">
-        <v>586532.1398948386</v>
+        <v>5.268907858948628</v>
       </c>
       <c r="K199">
-        <v>6825944.81658633</v>
+        <v>52.32875737333558</v>
       </c>
     </row>
     <row r="200" spans="1:11">
@@ -8589,10 +8589,10 @@
         <v>443</v>
       </c>
       <c r="J200">
-        <v>598055.834047391</v>
+        <v>5.372426964816193</v>
       </c>
       <c r="K200">
-        <v>6836712.729917548</v>
+        <v>52.38798075401587</v>
       </c>
     </row>
     <row r="201" spans="1:11">
@@ -8618,10 +8618,10 @@
         <v>444</v>
       </c>
       <c r="J201">
-        <v>598055.8307490128</v>
+        <v>5.372426935186358</v>
       </c>
       <c r="K201">
-        <v>6836729.081956357</v>
+        <v>52.3880706293583</v>
       </c>
     </row>
     <row r="202" spans="1:11">
@@ -8647,10 +8647,10 @@
         <v>445</v>
       </c>
       <c r="J202">
-        <v>596726.3337596373</v>
+        <v>5.360483860528889</v>
       </c>
       <c r="K202">
-        <v>6836933.107475961</v>
+        <v>52.38919199476197</v>
       </c>
     </row>
     <row r="203" spans="1:11">
@@ -8676,10 +8676,10 @@
         <v>446</v>
       </c>
       <c r="J203">
-        <v>596727.969006476</v>
+        <v>5.360498550201175</v>
       </c>
       <c r="K203">
-        <v>6836933.108075241</v>
+        <v>52.38919199805569</v>
       </c>
     </row>
     <row r="204" spans="1:11">
@@ -8705,10 +8705,10 @@
         <v>447</v>
       </c>
       <c r="J204">
-        <v>605535.8116705157</v>
+        <v>5.439620747053444</v>
       </c>
       <c r="K204">
-        <v>6826227.763510216</v>
+        <v>52.33031459826143</v>
       </c>
     </row>
     <row r="205" spans="1:11">
@@ -8734,10 +8734,10 @@
         <v>448</v>
       </c>
       <c r="J205">
-        <v>605535.8104855964</v>
+        <v>5.439620736409132</v>
       </c>
       <c r="K205">
-        <v>6826226.130432984</v>
+        <v>52.33030561062583</v>
       </c>
     </row>
     <row r="206" spans="1:11">
@@ -8763,10 +8763,10 @@
         <v>449</v>
       </c>
       <c r="J206">
-        <v>600115.7141596015</v>
+        <v>5.390931182698719</v>
       </c>
       <c r="K206">
-        <v>6827879.453226768</v>
+        <v>52.33940372803456</v>
       </c>
     </row>
     <row r="207" spans="1:11">
@@ -8792,10 +8792,10 @@
         <v>450</v>
       </c>
       <c r="J207">
-        <v>600114.0807472114</v>
+        <v>5.390916509505566</v>
       </c>
       <c r="K207">
-        <v>6827879.453314338</v>
+        <v>52.33940372851641</v>
       </c>
     </row>
     <row r="208" spans="1:11">
@@ -8821,10 +8821,10 @@
         <v>451</v>
       </c>
       <c r="J208">
-        <v>593021.3229984895</v>
+        <v>5.327201182583226</v>
       </c>
       <c r="K208">
-        <v>6828461.497419653</v>
+        <v>52.34260622806811</v>
       </c>
     </row>
     <row r="209" spans="1:11">
@@ -8850,10 +8850,10 @@
         <v>452</v>
       </c>
       <c r="J209">
-        <v>593022.9565280195</v>
+        <v>5.327215856828666</v>
       </c>
       <c r="K209">
-        <v>6828461.498768406</v>
+        <v>52.3426062354889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>